<commit_message>
light updates after class 07/10
</commit_message>
<xml_diff>
--- a/notebooks/google_merch_store/df_merch_values_pre_encoding.xlsx
+++ b/notebooks/google_merch_store/df_merch_values_pre_encoding.xlsx
@@ -439,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A14"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,6 +453,11 @@
           <t>event_name</t>
         </is>
       </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>event_name_enc</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -460,6 +465,7 @@
           <t>add_payment_info</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -467,6 +473,7 @@
           <t>add_shipping_info</t>
         </is>
       </c>
+      <c r="B3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -474,6 +481,7 @@
           <t>add_to_cart</t>
         </is>
       </c>
+      <c r="B4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -481,6 +489,7 @@
           <t>begin_checkout</t>
         </is>
       </c>
+      <c r="B5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -488,6 +497,7 @@
           <t>page_view</t>
         </is>
       </c>
+      <c r="B6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -495,6 +505,7 @@
           <t>purchase</t>
         </is>
       </c>
+      <c r="B7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -502,6 +513,7 @@
           <t>scroll</t>
         </is>
       </c>
+      <c r="B8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -509,6 +521,7 @@
           <t>select_item</t>
         </is>
       </c>
+      <c r="B9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -516,6 +529,7 @@
           <t>select_promotion</t>
         </is>
       </c>
+      <c r="B10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -523,6 +537,7 @@
           <t>user_engagement</t>
         </is>
       </c>
+      <c r="B11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -530,6 +545,7 @@
           <t>view_item</t>
         </is>
       </c>
+      <c r="B12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -537,6 +553,7 @@
           <t>view_promotion</t>
         </is>
       </c>
+      <c r="B13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -544,6 +561,7 @@
           <t>view_search_results</t>
         </is>
       </c>
+      <c r="B14" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -556,7 +574,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -570,6 +588,11 @@
           <t>geo_country</t>
         </is>
       </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>geo_country_enc</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -577,6 +600,7 @@
           <t>Canada</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -584,6 +608,7 @@
           <t>United States</t>
         </is>
       </c>
+      <c r="B3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -596,7 +621,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -610,6 +635,11 @@
           <t>traffic_source_medium</t>
         </is>
       </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>traffic_source_medium_enc</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -617,6 +647,7 @@
           <t>&lt;Other&gt;</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -624,6 +655,7 @@
           <t>cpc</t>
         </is>
       </c>
+      <c r="B3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -631,6 +663,7 @@
           <t>direct</t>
         </is>
       </c>
+      <c r="B4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -638,6 +671,7 @@
           <t>organic</t>
         </is>
       </c>
+      <c r="B5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -645,6 +679,7 @@
           <t>referral</t>
         </is>
       </c>
+      <c r="B6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -657,7 +692,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -671,6 +706,11 @@
           <t>traffic_source_source</t>
         </is>
       </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>traffic_source_source_enc</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -678,6 +718,7 @@
           <t>&lt;Other&gt;</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -685,6 +726,7 @@
           <t>direct</t>
         </is>
       </c>
+      <c r="B3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -692,6 +734,7 @@
           <t>google</t>
         </is>
       </c>
+      <c r="B4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -699,6 +742,7 @@
           <t>referral_link</t>
         </is>
       </c>
+      <c r="B5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -711,7 +755,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A21"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -725,146 +769,187 @@
           <t>page_path_level_1</t>
         </is>
       </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>page_path_level_1_enc</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>black lives matter | google merchandise store</t>
-        </is>
-      </c>
+          <t>apparel | google merchandise store</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>checkout confirmation</t>
-        </is>
-      </c>
+          <t>black lives matter | google merchandise store</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>checkout review</t>
-        </is>
-      </c>
+          <t>checkout confirmation</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>checkout your information</t>
-        </is>
-      </c>
+          <t>checkout review</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>google greenesign</t>
-        </is>
-      </c>
+          <t>checkout your information</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>google merchandise store - forgot password</t>
-        </is>
-      </c>
+          <t>clearance</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>google merchandise store - reset password</t>
-        </is>
-      </c>
+          <t>google greenesign</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>google online store</t>
-        </is>
-      </c>
+          <t>google merchandise store - forgot password</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>google redesign</t>
-        </is>
-      </c>
+          <t>google merchandise store - reset password</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>google rmg redesign</t>
-        </is>
-      </c>
+          <t>google online store</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>google yellowesign</t>
-        </is>
-      </c>
+          <t>google redesign</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>home</t>
-        </is>
-      </c>
+          <t>google rmg redesign</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>payment method</t>
-        </is>
-      </c>
+          <t>google yellowesign</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>shopping cart</t>
-        </is>
-      </c>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>store search results</t>
-        </is>
-      </c>
+          <t>payment method</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>store-policies</t>
-        </is>
-      </c>
+          <t>shopping cart</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>the google merchandise store - log in</t>
-        </is>
-      </c>
+          <t>store search results</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>the google merchandise store - my account</t>
-        </is>
-      </c>
+          <t>store-policies</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>the google merchandise store - register</t>
-        </is>
-      </c>
+          <t>the google merchandise store - log in</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
+          <t>the google merchandise store - my account</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>the google merchandise store - register</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
           <t>your wishlist</t>
         </is>
       </c>
+      <c r="B23" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -877,7 +962,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A54"/>
+  <dimension ref="A1:B55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -891,6 +976,11 @@
           <t>page_path_level_2</t>
         </is>
       </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>page_path_level_2_enc</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -898,370 +988,431 @@
           <t>&lt;NA&gt;/google redesign</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>black lives matter | google merchandise store</t>
-        </is>
-      </c>
+          <t>apparel | google merchandise store</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>checkout confirmation</t>
-        </is>
-      </c>
+          <t>black lives matter | google merchandise store</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>checkout review</t>
-        </is>
-      </c>
+          <t>checkout confirmation</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>checkout your information</t>
-        </is>
-      </c>
+          <t>checkout review</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>google greenesign/apparel</t>
-        </is>
-      </c>
+          <t>checkout your information</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>google merchandise store - forgot password</t>
-        </is>
-      </c>
+          <t>clearance/clearance-accessories</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>google merchandise store - reset password</t>
-        </is>
-      </c>
+          <t>google greenesign/apparel</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>google online store</t>
-        </is>
-      </c>
+          <t>google merchandise store - forgot password</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>google redesign/5k run</t>
-        </is>
-      </c>
+          <t>google merchandise store - reset password</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>google redesign/accessories</t>
-        </is>
-      </c>
+          <t>google online store</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>google redesign/apparel</t>
-        </is>
-      </c>
+          <t>google redesign/5k run</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>google redesign/apparelgoogle beekeepers tee mint</t>
-        </is>
-      </c>
+          <t>google redesign/accessories</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>google redesign/bags</t>
-        </is>
-      </c>
+          <t>google redesign/apparel</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>google redesign/blm unisex pullover hoodie</t>
-        </is>
-      </c>
+          <t>google redesign/apparelgoogle beekeepers tee mint</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>google redesign/campus collection</t>
-        </is>
-      </c>
+          <t>google redesign/bags</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>google redesign/clearance</t>
-        </is>
-      </c>
+          <t>google redesign/blm unisex pullover hoodie</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>google redesign/drinkware</t>
-        </is>
-      </c>
+          <t>google redesign/campus collection</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>google redesign/eco friendly</t>
-        </is>
-      </c>
+          <t>google redesign/clearance</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>google redesign/electronics</t>
-        </is>
-      </c>
+          <t>google redesign/drinkware</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>google redesign/gift cards</t>
-        </is>
-      </c>
+          <t>google redesign/eco friendly</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>google redesign/google blue stojo cup</t>
-        </is>
-      </c>
+          <t>google redesign/electronics</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>google redesign/google chrome dino light up water bottle</t>
-        </is>
-      </c>
+          <t>google redesign/gift cards</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>google redesign/google crew sweater navy</t>
-        </is>
-      </c>
+          <t>google redesign/google blue stojo cup</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>google redesign/google land and sea french terry sweatshirt</t>
-        </is>
-      </c>
+          <t>google redesign/google chrome dino light up water bottle</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>google redesign/google land and sea french terry sweatshirt ls</t>
-        </is>
-      </c>
+          <t>google redesign/google crew sweater navy</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>google redesign/google land and sea mug</t>
-        </is>
-      </c>
+          <t>google redesign/google land and sea french terry sweatshirt</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>google redesign/google land and sea mug ls</t>
-        </is>
-      </c>
+          <t>google redesign/google land and sea mug</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>google redesign/google land and sea tech taco</t>
-        </is>
-      </c>
+          <t>google redesign/google land and sea mug ls</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle</t>
-        </is>
-      </c>
+          <t>google redesign/google land and sea tech taco</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>google redesign/new</t>
-        </is>
-      </c>
+          <t>google redesign/lifestyle</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>google redesign/notebooks journals</t>
-        </is>
-      </c>
+          <t>google redesign/new</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>google redesign/office</t>
-        </is>
-      </c>
+          <t>google redesign/notebooks journals</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>google redesign/shop by brand</t>
-        </is>
-      </c>
+          <t>google redesign/office</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>google redesign/small goods</t>
-        </is>
-      </c>
+          <t>google redesign/shop by brand</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>google redesign/stationery</t>
-        </is>
-      </c>
+          <t>google redesign/small goods</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>google redesign/super g unisex joggers</t>
-        </is>
-      </c>
+          <t>google redesign/stationery</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>google redesign/wearables</t>
-        </is>
-      </c>
+          <t>google redesign/super g unisex joggers</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>google rmg redesign/lifestyle</t>
-        </is>
-      </c>
+          <t>google redesign/wearables</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>google yellowesign/apparel</t>
-        </is>
-      </c>
+          <t>google rmg redesign/lifestyle</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>home</t>
-        </is>
-      </c>
+          <t>google yellowesign/apparel</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>payment method</t>
-        </is>
-      </c>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>shopping cart</t>
-        </is>
-      </c>
+          <t>payment method</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>store search results</t>
-        </is>
-      </c>
+          <t>shopping cart</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>store-policies/frequently-asked-questions</t>
-        </is>
-      </c>
+          <t>store search results</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>store-policies/privacy-policy</t>
-        </is>
-      </c>
+          <t>store-policies/frequently-asked-questions</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>store-policies/return-policy</t>
-        </is>
-      </c>
+          <t>store-policies/privacy-policy</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>store-policies/shipping-information</t>
-        </is>
-      </c>
+          <t>store-policies/return-policy</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>store-policies/terms-of-use</t>
-        </is>
-      </c>
+          <t>store-policies/shipping-information</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>the google merchandise store - log in</t>
-        </is>
-      </c>
+          <t>store-policies/terms-of-use</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>the google merchandise store - my account</t>
-        </is>
-      </c>
+          <t>the google merchandise store - log in</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>the google merchandise store - register</t>
-        </is>
-      </c>
+          <t>the google merchandise store - my account</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
+          <t>the google merchandise store - register</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
           <t>your wishlist</t>
         </is>
       </c>
+      <c r="B55" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1274,7 +1425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A138"/>
+  <dimension ref="A1:B138"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1288,6 +1439,11 @@
           <t>page_path_level_3</t>
         </is>
       </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>page_path_level_3_enc</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1295,657 +1451,751 @@
           <t>&lt;NA&gt;/google redesign/office</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>black lives matter | google merchandise store</t>
-        </is>
-      </c>
+          <t>apparel | google merchandise store</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>checkout confirmation</t>
-        </is>
-      </c>
+          <t>black lives matter | google merchandise store</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>checkout review</t>
-        </is>
-      </c>
+          <t>checkout confirmation</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>checkout your information</t>
-        </is>
-      </c>
+          <t>checkout review</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>google greenesign/apparel/other</t>
-        </is>
-      </c>
+          <t>checkout your information</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>google merchandise store - forgot password</t>
-        </is>
-      </c>
+          <t>clearance/clearance-accessories</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>google merchandise store - reset password</t>
-        </is>
-      </c>
+          <t>google greenesign/apparel/other</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>google online store</t>
-        </is>
-      </c>
+          <t>google merchandise store - forgot password</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>google redesign/5k run/other</t>
-        </is>
-      </c>
+          <t>google merchandise store - reset password</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>google redesign/accessories</t>
-        </is>
-      </c>
+          <t>google online store</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google campus bike</t>
-        </is>
-      </c>
+          <t>google redesign/5k run/other</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google chrome dinosaur collectible</t>
-        </is>
-      </c>
+          <t>google redesign/accessories</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google pride sticker</t>
-        </is>
-      </c>
+          <t>google redesign/accessories/google campus bike</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>google redesign/accessories/noogler android figure 2019</t>
-        </is>
-      </c>
+          <t>google redesign/accessories/google chrome dinosaur collectible</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>google redesign/accessories/other</t>
-        </is>
-      </c>
+          <t>google redesign/accessories/noogler android figure 2019</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>google redesign/apparel</t>
-        </is>
-      </c>
+          <t>google redesign/accessories/other</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android garden tee orange</t>
-        </is>
-      </c>
+          <t>google redesign/apparel</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android iconic beanie</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/android garden tee orange</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android iconic hat green</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/android iconic beanie</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android iconic hat v2 black</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/android iconic hat green</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android iconic hat white</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/android iconic hat v2 black</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android iconic sock</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/android iconic hat white</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google badge heavyweight pullover black</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/android iconic sock</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google black tee</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/google badge heavyweight pullover black</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google campus bike eco tee navy</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/google black tee</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google cotopaxi shell</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/google campus bike eco tee navy</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google crew socks</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/google cotopaxi shell</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google crewneck sweatshirt green</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/google crew socks</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google dino game tee</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/google crewneck sweatshirt green</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google fc longsleeve ash</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/google dino game tee</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google fc longsleeve charcoal</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/google fc longsleeve ash</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google google crew combed cotton sock</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/google fc longsleeve charcoal</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google google crew striped athletic sock</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/google google crew combed cotton sock</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google heather green speckled tee</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/google google crew striped athletic sock</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google heathered pom beanie</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/google heather green speckled tee</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google infant charcoal onesie</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/google heathered pom beanie</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google infant hero tee olive</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/google infant charcoal onesie</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google land and sea cotton cap ls</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/google infant hero tee olive</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google land and sea unisex tee</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/google land and sea cotton cap ls</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google land and sea womens eco tee</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/google land and sea unisex tee</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google leather strap hat black</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/google land and sea womens eco tee</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google leather strap hat blue</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/google leather strap hat black</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google mural socks</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/google leather strap hat blue</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google navy speckled tee</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/google mens puff jacket black</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google sherpa zip hoodie charcoal</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/google mural socks</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google sherpa zip hoodie navy</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/google navy speckled tee</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google speckled beanie grey</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/google sherpa zip hoodie charcoal</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google speckled beanie navy</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/google sherpa zip hoodie navy</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google tee fc black</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/google speckled beanie grey</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google toddler fc tee charcoal</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/google speckled beanie navy</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google toddler fc zip hoodie</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/google tee fc black</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google toddler tee white</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/google toddler fc tee charcoal</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google unisex eco tee black</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/google toddler fc zip hoodie</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens google striped ls</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/google toddler tee white</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens grid zip up</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/google unisex eco tee black</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens microfleece jacket black</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/google womens google striped ls</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens puff jacket black</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/google womens grid zip up</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google youth fc longsleeve charcoal</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/google womens microfleece jacket black</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google youth fc tee charcoal</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/google womens puff jacket black</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google youth hero tee grey</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/google youth fc longsleeve charcoal</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google zip hoodie fc</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/google youth fc tee charcoal</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>google redesign/apparel/hats</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/google youth hero tee grey</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>google redesign/apparel/iamremarkable hoodie</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/google zip hoodie fc</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>google redesign/apparel/iamremarkable ladies t-shirt</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/hats</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>google redesign/apparel/other</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/iamremarkable hoodie</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>google redesign/apparel/socks</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/iamremarkable ladies t-shirt</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>google redesign/apparel/stan and friends tee green</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/other</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>google redesign/apparel/youtube crew socks</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/socks</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>google redesign/apparel/youtube icon hoodie black</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/youtube crew socks</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>google redesign/apparel/youtube leather strap hat black</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/youtube icon hoodie black</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>google redesign/apparel/youtube twill cap sandwich black</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/youtube icon tee grey</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>google redesign/apparelgoogle beekeepers tee mint</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/youtube leather strap hat black</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>google redesign/bags/backpacks</t>
-        </is>
-      </c>
+          <t>google redesign/apparel/youtube twill cap sandwich black</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>google redesign/bags/google flat front bag grey</t>
-        </is>
-      </c>
+          <t>google redesign/apparelgoogle beekeepers tee mint</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>google redesign/bags/google incognito zippack v2</t>
-        </is>
-      </c>
+          <t>google redesign/bags/backpacks</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>google redesign/bags/google utility backpack</t>
-        </is>
-      </c>
+          <t>google redesign/bags/google flat front bag grey</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>google redesign/bags/other</t>
-        </is>
-      </c>
+          <t>google redesign/bags/google incognito zippack v2</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>google redesign/blm unisex pullover hoodie</t>
-        </is>
-      </c>
+          <t>google redesign/bags/google utility backpack</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>google redesign/campus collection</t>
-        </is>
-      </c>
+          <t>google redesign/bags/other</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>google redesign/campus collection/other</t>
-        </is>
-      </c>
+          <t>google redesign/blm unisex pullover hoodie</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>google redesign/clearance</t>
-        </is>
-      </c>
+          <t>google redesign/campus collection</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/mugs tumblers</t>
-        </is>
-      </c>
+          <t>google redesign/campus collection/other</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/other</t>
-        </is>
-      </c>
+          <t>google redesign/clearance</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/water bottles</t>
-        </is>
-      </c>
+          <t>google redesign/drinkware/mugs tumblers</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>google redesign/eco friendly</t>
-        </is>
-      </c>
+          <t>google redesign/drinkware/other</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>google redesign/electronics</t>
-        </is>
-      </c>
+          <t>google redesign/drinkware/water bottles</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>google redesign/electronics/other</t>
-        </is>
-      </c>
+          <t>google redesign/eco friendly</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>google redesign/gift cards</t>
-        </is>
-      </c>
+          <t>google redesign/electronics/other</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>google redesign/google blue stojo cup</t>
-        </is>
-      </c>
+          <t>google redesign/gift cards</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>google redesign/google chrome dino light up water bottle</t>
-        </is>
-      </c>
+          <t>google redesign/google blue stojo cup</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>google redesign/google crew sweater navy</t>
-        </is>
-      </c>
+          <t>google redesign/google chrome dino light up water bottle</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>google redesign/google land and sea french terry sweatshirt</t>
-        </is>
-      </c>
+          <t>google redesign/google crew sweater navy</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>google redesign/google land and sea french terry sweatshirt ls</t>
-        </is>
-      </c>
+          <t>google redesign/google land and sea french terry sweatshirt</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -1953,6 +2203,7 @@
           <t>google redesign/google land and sea mug</t>
         </is>
       </c>
+      <c r="B96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -1960,6 +2211,7 @@
           <t>google redesign/google land and sea mug ls</t>
         </is>
       </c>
+      <c r="B97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -1967,6 +2219,7 @@
           <t>google redesign/google land and sea tech taco</t>
         </is>
       </c>
+      <c r="B98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -1974,6 +2227,7 @@
           <t>google redesign/lifestyle</t>
         </is>
       </c>
+      <c r="B99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -1981,6 +2235,7 @@
           <t>google redesign/lifestyle/bags</t>
         </is>
       </c>
+      <c r="B100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -1988,62 +2243,71 @@
           <t>google redesign/lifestyle/drinkware</t>
         </is>
       </c>
+      <c r="B101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/google land and sea nalgene water bottle ls</t>
-        </is>
-      </c>
+          <t>google redesign/lifestyle/google bear baby blanket beige</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/google land and sea tote bag</t>
-        </is>
-      </c>
+          <t>google redesign/lifestyle/google land and sea nalgene water bottle ls</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/other</t>
-        </is>
-      </c>
+          <t>google redesign/lifestyle/google land and sea tote bag</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/small goods</t>
-        </is>
-      </c>
+          <t>google redesign/lifestyle/other</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>google redesign/new</t>
-        </is>
-      </c>
+          <t>google redesign/lifestyle/small goods</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>google redesign/notebooks journals/other</t>
-        </is>
-      </c>
+          <t>google redesign/new</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>google redesign/office</t>
-        </is>
-      </c>
+          <t>google redesign/notebooks journals/other</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>google redesign/office/google phone stand bamboo</t>
-        </is>
-      </c>
+          <t>google redesign/office</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -2051,6 +2315,7 @@
           <t>google redesign/office/other</t>
         </is>
       </c>
+      <c r="B110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -2058,6 +2323,7 @@
           <t>google redesign/shop by brand</t>
         </is>
       </c>
+      <c r="B111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -2065,6 +2331,7 @@
           <t>google redesign/shop by brand/android</t>
         </is>
       </c>
+      <c r="B112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -2072,6 +2339,7 @@
           <t>google redesign/shop by brand/google</t>
         </is>
       </c>
+      <c r="B113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -2079,6 +2347,7 @@
           <t>google redesign/shop by brand/google cloud</t>
         </is>
       </c>
+      <c r="B114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -2086,6 +2355,7 @@
           <t>google redesign/shop by brand/i am remarkable</t>
         </is>
       </c>
+      <c r="B115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -2093,6 +2363,7 @@
           <t>google redesign/shop by brand/youtube</t>
         </is>
       </c>
+      <c r="B116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -2100,6 +2371,7 @@
           <t>google redesign/small goods/other</t>
         </is>
       </c>
+      <c r="B117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -2107,6 +2379,7 @@
           <t>google redesign/stationery</t>
         </is>
       </c>
+      <c r="B118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -2114,6 +2387,7 @@
           <t>google redesign/stationery/google land and sea journal set</t>
         </is>
       </c>
+      <c r="B119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -2121,6 +2395,7 @@
           <t>google redesign/stationery/notebooks</t>
         </is>
       </c>
+      <c r="B120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -2128,6 +2403,7 @@
           <t>google redesign/stationery/other</t>
         </is>
       </c>
+      <c r="B121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -2135,13 +2411,15 @@
           <t>google redesign/super g unisex joggers</t>
         </is>
       </c>
+      <c r="B122" t="inlineStr"/>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>google redesign/wearables/men s t-shirts</t>
-        </is>
-      </c>
+          <t>google redesign/wearables/other</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -2149,6 +2427,7 @@
           <t>google rmg redesign/lifestyle/mural food container</t>
         </is>
       </c>
+      <c r="B124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -2156,6 +2435,7 @@
           <t>google yellowesign/apparel/other</t>
         </is>
       </c>
+      <c r="B125" t="inlineStr"/>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -2163,6 +2443,7 @@
           <t>home</t>
         </is>
       </c>
+      <c r="B126" t="inlineStr"/>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -2170,6 +2451,7 @@
           <t>payment method</t>
         </is>
       </c>
+      <c r="B127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -2177,6 +2459,7 @@
           <t>shopping cart</t>
         </is>
       </c>
+      <c r="B128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -2184,6 +2467,7 @@
           <t>store search results</t>
         </is>
       </c>
+      <c r="B129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -2191,6 +2475,7 @@
           <t>store-policies/frequently-asked-questions</t>
         </is>
       </c>
+      <c r="B130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -2198,6 +2483,7 @@
           <t>store-policies/privacy-policy</t>
         </is>
       </c>
+      <c r="B131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -2205,6 +2491,7 @@
           <t>store-policies/return-policy</t>
         </is>
       </c>
+      <c r="B132" t="inlineStr"/>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -2212,6 +2499,7 @@
           <t>store-policies/shipping-information</t>
         </is>
       </c>
+      <c r="B133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -2219,6 +2507,7 @@
           <t>store-policies/terms-of-use</t>
         </is>
       </c>
+      <c r="B134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -2226,6 +2515,7 @@
           <t>the google merchandise store - log in</t>
         </is>
       </c>
+      <c r="B135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -2233,6 +2523,7 @@
           <t>the google merchandise store - my account</t>
         </is>
       </c>
+      <c r="B136" t="inlineStr"/>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -2240,6 +2531,7 @@
           <t>the google merchandise store - register</t>
         </is>
       </c>
+      <c r="B137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -2247,6 +2539,7 @@
           <t>your wishlist</t>
         </is>
       </c>
+      <c r="B138" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2259,7 +2552,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2273,6 +2566,11 @@
           <t>device_category</t>
         </is>
       </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>device_category_enc</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -2280,6 +2578,7 @@
           <t>desktop</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -2287,6 +2586,7 @@
           <t>mobile</t>
         </is>
       </c>
+      <c r="B3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -2294,6 +2594,7 @@
           <t>tablet</t>
         </is>
       </c>
+      <c r="B4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2306,7 +2607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2320,6 +2621,11 @@
           <t>device_mobile_brand_name</t>
         </is>
       </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>device_mobile_brand_name_enc</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -2327,6 +2633,7 @@
           <t>&lt;Other&gt;</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -2334,6 +2641,7 @@
           <t>Apple</t>
         </is>
       </c>
+      <c r="B3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -2341,6 +2649,7 @@
           <t>Google</t>
         </is>
       </c>
+      <c r="B4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -2348,6 +2657,7 @@
           <t>Huawei</t>
         </is>
       </c>
+      <c r="B5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -2355,6 +2665,7 @@
           <t>Microsoft</t>
         </is>
       </c>
+      <c r="B6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -2362,6 +2673,7 @@
           <t>Mozilla</t>
         </is>
       </c>
+      <c r="B7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -2369,6 +2681,7 @@
           <t>PC</t>
         </is>
       </c>
+      <c r="B8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -2376,6 +2689,7 @@
           <t>Samsung</t>
         </is>
       </c>
+      <c r="B9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -2383,6 +2697,7 @@
           <t>Xiaomi</t>
         </is>
       </c>
+      <c r="B10" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2395,7 +2710,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A21"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2409,6 +2724,11 @@
           <t>device_mobile_model_name</t>
         </is>
       </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>device_mobile_model_name_enc</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -2416,90 +2736,103 @@
           <t>&lt;Other&gt; - &lt;Other&gt;</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>&lt;Other&gt; - Edge</t>
-        </is>
-      </c>
+          <t>Apple - Macintosh</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Apple - Macintosh</t>
-        </is>
-      </c>
+          <t>Apple - iPad</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Apple - iPad</t>
-        </is>
-      </c>
+          <t>Apple - iPhone</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Apple - iPhone</t>
-        </is>
-      </c>
+          <t>Google - &lt;Other&gt;</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Google - &lt;Other&gt;</t>
-        </is>
-      </c>
+          <t>Google - Chrome</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Google - Chrome</t>
-        </is>
-      </c>
+          <t>Google - ChromeBook</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Google - ChromeBook</t>
-        </is>
-      </c>
+          <t>Google - Pixel 3</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Google - Pixel 3</t>
-        </is>
-      </c>
+          <t>Google - Pixel 4 XL</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Google - Pixel 4 XL</t>
-        </is>
-      </c>
+          <t>Huawei - &lt;Other&gt;</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Huawei - &lt;Other&gt;</t>
-        </is>
-      </c>
+          <t>Huawei - P50</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Huawei - P50</t>
-        </is>
-      </c>
+          <t>Microsoft - &lt;Other&gt;</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Microsoft - &lt;Other&gt;</t>
-        </is>
-      </c>
+          <t>Mozilla - &lt;Other&gt;</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2507,6 +2840,7 @@
           <t>Mozilla - Firefox</t>
         </is>
       </c>
+      <c r="B15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2514,6 +2848,7 @@
           <t>PC - &lt;Other&gt;</t>
         </is>
       </c>
+      <c r="B16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2521,6 +2856,7 @@
           <t>PC - Edge</t>
         </is>
       </c>
+      <c r="B17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2528,6 +2864,7 @@
           <t>PC - Firefox</t>
         </is>
       </c>
+      <c r="B18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2535,6 +2872,7 @@
           <t>PC - PC</t>
         </is>
       </c>
+      <c r="B19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2542,6 +2880,7 @@
           <t>Samsung - Galaxy S21</t>
         </is>
       </c>
+      <c r="B20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2549,6 +2888,7 @@
           <t>Xiaomi - Mi 11</t>
         </is>
       </c>
+      <c r="B21" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2561,7 +2901,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2575,6 +2915,11 @@
           <t>device_language</t>
         </is>
       </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>device_language_enc</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -2582,6 +2927,7 @@
           <t>de</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -2589,6 +2935,7 @@
           <t>en</t>
         </is>
       </c>
+      <c r="B3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -2596,6 +2943,7 @@
           <t>en-ca</t>
         </is>
       </c>
+      <c r="B4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -2603,6 +2951,7 @@
           <t>en-gb</t>
         </is>
       </c>
+      <c r="B5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -2610,6 +2959,7 @@
           <t>en-us</t>
         </is>
       </c>
+      <c r="B6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -2617,6 +2967,7 @@
           <t>es-es</t>
         </is>
       </c>
+      <c r="B7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -2624,6 +2975,7 @@
           <t>fr</t>
         </is>
       </c>
+      <c r="B8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -2631,6 +2983,7 @@
           <t>ko</t>
         </is>
       </c>
+      <c r="B9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -2638,6 +2991,7 @@
           <t>zh</t>
         </is>
       </c>
+      <c r="B10" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2650,7 +3004,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A16"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2664,6 +3018,11 @@
           <t>device_operating_system_version</t>
         </is>
       </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>device_operating_system_version_enc</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -2671,6 +3030,7 @@
           <t xml:space="preserve">&lt;Other&gt; - </t>
         </is>
       </c>
+      <c r="B2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -2678,6 +3038,7 @@
           <t xml:space="preserve">Android - </t>
         </is>
       </c>
+      <c r="B3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -2685,6 +3046,7 @@
           <t>Android - 10</t>
         </is>
       </c>
+      <c r="B4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -2692,6 +3054,7 @@
           <t>Android - 9</t>
         </is>
       </c>
+      <c r="B5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -2699,6 +3062,7 @@
           <t xml:space="preserve">MacOS - </t>
         </is>
       </c>
+      <c r="B6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -2706,6 +3070,7 @@
           <t>MacOS - 10.15</t>
         </is>
       </c>
+      <c r="B7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -2713,6 +3078,7 @@
           <t>MacOS - 11.1</t>
         </is>
       </c>
+      <c r="B8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -2720,6 +3086,7 @@
           <t xml:space="preserve">Web - </t>
         </is>
       </c>
+      <c r="B9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -2727,6 +3094,7 @@
           <t>Web - 10</t>
         </is>
       </c>
+      <c r="B10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -2734,6 +3102,7 @@
           <t xml:space="preserve">Windows - </t>
         </is>
       </c>
+      <c r="B11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -2741,6 +3110,7 @@
           <t>Windows - 10</t>
         </is>
       </c>
+      <c r="B12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2748,6 +3118,7 @@
           <t>Windows - 7</t>
         </is>
       </c>
+      <c r="B13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2755,6 +3126,7 @@
           <t xml:space="preserve">iOS - </t>
         </is>
       </c>
+      <c r="B14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2762,6 +3134,7 @@
           <t>iOS - 14.2</t>
         </is>
       </c>
+      <c r="B15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2769,6 +3142,7 @@
           <t>iOS - 14.3</t>
         </is>
       </c>
+      <c r="B16" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2781,7 +3155,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2795,6 +3169,11 @@
           <t>device_operating_system</t>
         </is>
       </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>device_operating_system_enc</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -2802,6 +3181,7 @@
           <t>&lt;Other&gt;</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -2809,6 +3189,7 @@
           <t>Android</t>
         </is>
       </c>
+      <c r="B3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -2816,6 +3197,7 @@
           <t>MacOS</t>
         </is>
       </c>
+      <c r="B4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -2823,6 +3205,7 @@
           <t>Web</t>
         </is>
       </c>
+      <c r="B5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -2830,6 +3213,7 @@
           <t>Windows</t>
         </is>
       </c>
+      <c r="B6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -2837,6 +3221,7 @@
           <t>iOS</t>
         </is>
       </c>
+      <c r="B7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2849,7 +3234,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2863,6 +3248,11 @@
           <t>device_web_info_browser</t>
         </is>
       </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>device_web_info_browser_enc</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -2870,6 +3260,7 @@
           <t>&lt;Other&gt;</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -2877,6 +3268,7 @@
           <t>Chrome</t>
         </is>
       </c>
+      <c r="B3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -2884,6 +3276,7 @@
           <t>Edge</t>
         </is>
       </c>
+      <c r="B4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -2891,6 +3284,7 @@
           <t>Firefox</t>
         </is>
       </c>
+      <c r="B5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -2898,6 +3292,7 @@
           <t>Safari</t>
         </is>
       </c>
+      <c r="B6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2910,7 +3305,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A20"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2924,6 +3319,11 @@
           <t>device_web_info_browser_version</t>
         </is>
       </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>device_web_info_browser_version_enc</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -2931,6 +3331,7 @@
           <t>&lt;Other&gt; - &lt;Other&gt;</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -2938,6 +3339,7 @@
           <t>Chrome - 86</t>
         </is>
       </c>
+      <c r="B3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -2945,6 +3347,7 @@
           <t>Chrome - 86.0</t>
         </is>
       </c>
+      <c r="B4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -2952,6 +3355,7 @@
           <t>Chrome - 87</t>
         </is>
       </c>
+      <c r="B5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -2959,6 +3363,7 @@
           <t>Chrome - 87.0</t>
         </is>
       </c>
+      <c r="B6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -2966,6 +3371,7 @@
           <t>Chrome - &lt;Other&gt;</t>
         </is>
       </c>
+      <c r="B7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -2973,6 +3379,7 @@
           <t>Edge - 86.0</t>
         </is>
       </c>
+      <c r="B8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -2980,6 +3387,7 @@
           <t>Edge - 87.0</t>
         </is>
       </c>
+      <c r="B9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -2987,6 +3395,7 @@
           <t>Edge - &lt;Other&gt;</t>
         </is>
       </c>
+      <c r="B10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -2994,6 +3403,7 @@
           <t>Firefox - 82.0</t>
         </is>
       </c>
+      <c r="B11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -3001,6 +3411,7 @@
           <t>Firefox - 83.0</t>
         </is>
       </c>
+      <c r="B12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -3008,6 +3419,7 @@
           <t>Firefox - 84.0</t>
         </is>
       </c>
+      <c r="B13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -3015,6 +3427,7 @@
           <t>Firefox - &lt;Other&gt;</t>
         </is>
       </c>
+      <c r="B14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -3022,6 +3435,7 @@
           <t>Safari - 13.0</t>
         </is>
       </c>
+      <c r="B15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -3029,6 +3443,7 @@
           <t>Safari - 13.1</t>
         </is>
       </c>
+      <c r="B16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -3036,6 +3451,7 @@
           <t>Safari - 14.0</t>
         </is>
       </c>
+      <c r="B17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -3043,6 +3459,7 @@
           <t>Safari - 14.1</t>
         </is>
       </c>
+      <c r="B18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -3050,6 +3467,7 @@
           <t>Safari - 604</t>
         </is>
       </c>
+      <c r="B19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -3057,6 +3475,7 @@
           <t>Safari - &lt;Other&gt;</t>
         </is>
       </c>
+      <c r="B20" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>